<commit_message>
Import von Mitarbeiterdaten mit neuer Datenbank mit Python aus moeglich!!!
</commit_message>
<xml_diff>
--- a/src/main/insert Entgeltdaten/1 Gewerkschaft.xlsx
+++ b/src/main/insert Entgeltdaten/1 Gewerkschaft.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\insert Entgeltdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA6D8B03-DB52-4AEF-842A-DDF434FEB51C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DD498D-5889-44B6-B8A6-ED826EFC7555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33945" yWindow="2880" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35115" yWindow="3390" windowWidth="17280" windowHeight="6780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -383,7 +383,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Unittests fuer die Methoden 'insert_unfallversicherungsbeitrag' und 'insert_gewerkschaft' geschrieben.
</commit_message>
<xml_diff>
--- a/src/main/insert Entgeltdaten/1 Gewerkschaft.xlsx
+++ b/src/main/insert Entgeltdaten/1 Gewerkschaft.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\insert Entgeltdaten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DD498D-5889-44B6-B8A6-ED826EFC7555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97FE48F-CC1D-46D6-A7DA-A2DA73F4A334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35115" yWindow="3390" windowWidth="17280" windowHeight="6780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3060" yWindow="2160" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Daten</t>
   </si>
@@ -47,12 +47,6 @@
   </si>
   <si>
     <t>Verdi</t>
-  </si>
-  <si>
-    <t>Branche</t>
-  </si>
-  <si>
-    <t>Drucktechnologie</t>
   </si>
 </sst>
 </file>
@@ -380,7 +374,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -408,14 +402,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
BAchelorarbeit: Kapitel 1 geschrieben.
</commit_message>
<xml_diff>
--- a/src/main/insert Entgeltdaten/1 Gewerkschaft.xlsx
+++ b/src/main/insert Entgeltdaten/1 Gewerkschaft.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\insert Entgeltdaten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\test\testdaten_insert_gewerkschaft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97FE48F-CC1D-46D6-A7DA-A2DA73F4A334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27DDE3E-6C20-4521-898D-A9555647D998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3060" yWindow="2160" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>